<commit_message>
feat: PoolManager and some UI logic(need refactor)
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excels/AttributeCardManual.xlsx
+++ b/Assets/Resources/Excels/AttributeCardManual.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Id</t>
   </si>
@@ -44,6 +44,9 @@
     <t>行动次数</t>
   </si>
   <si>
+    <t>目标数量</t>
+  </si>
+  <si>
     <t>描述</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t>ActionNum</t>
+  </si>
+  <si>
+    <t>TargetCount</t>
   </si>
   <si>
     <t>Description</t>
@@ -1023,22 +1029,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F3"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="10.425" style="1" customWidth="1"/>
     <col min="3" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="10.6833333333333" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="13.525" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6833333333333" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1057,78 +1064,96 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>